<commit_message>
Optimierungen/Fix für Stamina, StopBall und XML
</commit_message>
<xml_diff>
--- a/doc/UnrealCup_Meilensteinplan_Sem6.xlsx
+++ b/doc/UnrealCup_Meilensteinplan_Sem6.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +105,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -171,6 +184,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -454,7 +469,7 @@
   <dimension ref="A7:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,21 +528,22 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -565,29 +581,29 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -595,7 +611,7 @@
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>

</xml_diff>